<commit_message>
phyloseq and heatmap templates
</commit_message>
<xml_diff>
--- a/docs/eDNA 12S metab/example_output/Filtered_10_removed_reads.xlsx
+++ b/docs/eDNA 12S metab/example_output/Filtered_10_removed_reads.xlsx
@@ -10549,22 +10549,22 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>407f08a29007a8a153222d82ef47d408</t>
+          <t>1b650324aafac0e6e6f0c473eccff258</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E58">
@@ -10588,7 +10588,7 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -10726,22 +10726,22 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1b650324aafac0e6e6f0c473eccff258</t>
+          <t>407f08a29007a8a153222d82ef47d408</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E59">
@@ -10765,7 +10765,7 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -13735,22 +13735,22 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>d34820a8c9954e292ea9dbc76f4275b4</t>
+          <t>09351b480c58a99c4150d54ebbc97c6c</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E76">
@@ -13912,22 +13912,22 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>09351b480c58a99c4150d54ebbc97c6c</t>
+          <t>d34820a8c9954e292ea9dbc76f4275b4</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E77">
@@ -16744,22 +16744,22 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>4c5905c5ab539613d9c3069d0ae54188</t>
+          <t>680475954df3011ebba1033f1b2f2a86</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Bos taurus</t>
+          <t>Prionotus carolinus</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Cow</t>
+          <t>Northern sea robin</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E93">
@@ -16774,7 +16774,7 @@
         <v>0</v>
       </c>
       <c r="H93">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I93">
         <v>0</v>
@@ -16858,7 +16858,7 @@
         <v>0</v>
       </c>
       <c r="AJ93">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK93">
         <v>0</v>
@@ -16891,7 +16891,7 @@
         <v>0</v>
       </c>
       <c r="AU93">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AV93">
         <v>0</v>
@@ -16900,7 +16900,7 @@
         <v>0</v>
       </c>
       <c r="AX93">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AY93">
         <v>0</v>
@@ -16921,22 +16921,22 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>db8615250f29272019fe417d96bf08f3</t>
+          <t>4c5905c5ab539613d9c3069d0ae54188</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Bos taurus</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Cow</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E94">
@@ -16951,7 +16951,7 @@
         <v>0</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -17035,7 +17035,7 @@
         <v>0</v>
       </c>
       <c r="AJ94">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK94">
         <v>0</v>
@@ -17068,7 +17068,7 @@
         <v>0</v>
       </c>
       <c r="AU94">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AV94">
         <v>0</v>
@@ -17098,17 +17098,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>680475954df3011ebba1033f1b2f2a86</t>
+          <t>db8615250f29272019fe417d96bf08f3</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Prionotus carolinus</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Northern sea robin</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -17254,7 +17254,7 @@
         <v>0</v>
       </c>
       <c r="AX95">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AY95">
         <v>0</v>
@@ -18868,17 +18868,17 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>6d1668646cf923fa90217b0797de7a7d</t>
+          <t>f5e0ea6fe3e45da9605b758c440ae692</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -19045,17 +19045,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>f5e0ea6fe3e45da9605b758c440ae692</t>
+          <t>6d1668646cf923fa90217b0797de7a7d</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -20284,17 +20284,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>f524c4b860dec1e6b994c28dd8e4b75e</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Paralichthys dentatus</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Summer flounder</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -20368,7 +20368,7 @@
         <v>0</v>
       </c>
       <c r="Z113">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA113">
         <v>0</v>
@@ -20431,7 +20431,7 @@
         <v>0</v>
       </c>
       <c r="AU113">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AV113">
         <v>0</v>
@@ -20461,17 +20461,17 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>f524c4b860dec1e6b994c28dd8e4b75e</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Paralichthys dentatus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Summer flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -20545,7 +20545,7 @@
         <v>0</v>
       </c>
       <c r="Z114">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA114">
         <v>0</v>
@@ -20608,7 +20608,7 @@
         <v>0</v>
       </c>
       <c r="AU114">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AV114">
         <v>0</v>
@@ -25771,17 +25771,17 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0df37a1b74088f0e7410a1b78cada881</t>
+          <t>9db3dc01519672b43908456a37b27b4d</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Engraulis eurystole</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Silver anchovy</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -25900,7 +25900,7 @@
         <v>0</v>
       </c>
       <c r="AO144">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AP144">
         <v>0</v>
@@ -25948,17 +25948,17 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>9db3dc01519672b43908456a37b27b4d</t>
+          <t>0df37a1b74088f0e7410a1b78cada881</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Engraulis eurystole</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Silver anchovy</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -26077,7 +26077,7 @@
         <v>0</v>
       </c>
       <c r="AO145">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AP145">
         <v>0</v>
@@ -26833,7 +26833,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>94a944154183c458facbab20fe39ffa9</t>
+          <t>0f011be680aec3ee4b12b1b139902251</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -27010,7 +27010,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>0f011be680aec3ee4b12b1b139902251</t>
+          <t>94a944154183c458facbab20fe39ffa9</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -30727,17 +30727,17 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>148aa3594130e12c353383f68bfa0b6a</t>
+          <t>191ed810bb884ed43fa1919f6da3d82a</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -30904,17 +30904,17 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>191ed810bb884ed43fa1919f6da3d82a</t>
+          <t>148aa3594130e12c353383f68bfa0b6a</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -31081,17 +31081,17 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>ed00c11476e9a07d3441cb0a1073d3ab</t>
+          <t>c73cefb2b4ac8de08ae0c68341cbb28f</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Etropus microstomus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Smallmouth flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -31231,7 +31231,7 @@
         <v>0</v>
       </c>
       <c r="AV174">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AW174">
         <v>0</v>
@@ -31252,23 +31252,23 @@
         <v>0</v>
       </c>
       <c r="BC174">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>c73cefb2b4ac8de08ae0c68341cbb28f</t>
+          <t>ed00c11476e9a07d3441cb0a1073d3ab</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Etropus microstomus</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Smallmouth flounder</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -31408,7 +31408,7 @@
         <v>0</v>
       </c>
       <c r="AV175">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW175">
         <v>0</v>
@@ -31429,7 +31429,7 @@
         <v>0</v>
       </c>
       <c r="BC175">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -32320,17 +32320,17 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>558d8758ae62abe36b1507ce2094ef7c</t>
+          <t>ff405ebc8992c59ba51a99e33a12fe74</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -32497,17 +32497,17 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>ff405ebc8992c59ba51a99e33a12fe74</t>
+          <t>558d8758ae62abe36b1507ce2094ef7c</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -33205,17 +33205,17 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>86c340102750abe5f2a75f3d5501b55d</t>
+          <t>ee3c408644b66e62dde706ff463f359a</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Menidia beryllina</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Inland silverside</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -33382,17 +33382,17 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>ee3c408644b66e62dde706ff463f359a</t>
+          <t>86c340102750abe5f2a75f3d5501b55d</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Menidia beryllina</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Inland silverside</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -33913,17 +33913,17 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>8830d0cf4452e1cd0f9a6552b48b2b40</t>
+          <t>0ad9142dc74ab0ef2021cfff48d4194d</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -34090,17 +34090,17 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>0ad9142dc74ab0ef2021cfff48d4194d</t>
+          <t>8830d0cf4452e1cd0f9a6552b48b2b40</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -34267,17 +34267,17 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>f2e15a0b398b704a888c965d3b49035b</t>
+          <t>731abf4fa491ab03dd796729de5ab3eb</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -34798,17 +34798,17 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>731abf4fa491ab03dd796729de5ab3eb</t>
+          <t>f2e15a0b398b704a888c965d3b49035b</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -36568,22 +36568,22 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>1533469db84e906a7d07208d202f0b61</t>
+          <t>e468b57f39f048ada7562924022dc516</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E205">
@@ -36745,22 +36745,22 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>e468b57f39f048ada7562924022dc516</t>
+          <t>1533469db84e906a7d07208d202f0b61</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E206">
@@ -38515,22 +38515,22 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>bdb87097756f45aa57e56f1d9f456f26</t>
+          <t>5b2278535af7a77c15966bc43d0188bd</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Larus sp</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Great black backed gull and other gulls</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E216">
@@ -38692,17 +38692,17 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>5b2278535af7a77c15966bc43d0188bd</t>
+          <t>6a83eb23e34e01773abb7d038e38c583</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -38869,22 +38869,22 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>cb17be39fabe38eb2368ba0635321393</t>
+          <t>bdb87097756f45aa57e56f1d9f456f26</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Tautoga onitis</t>
+          <t>Larus sp</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Tautog</t>
+          <t>Great black backed gull and other gulls</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E218">
@@ -39223,22 +39223,22 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>c0b18824ab60460cd31eed51f737f882</t>
+          <t>cb17be39fabe38eb2368ba0635321393</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Tautoga onitis</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tautog</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E220">
@@ -39400,22 +39400,22 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>6a83eb23e34e01773abb7d038e38c583</t>
+          <t>c0b18824ab60460cd31eed51f737f882</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E221">
@@ -40108,17 +40108,17 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>f937641d91db232cb7180be9e04fb9e0</t>
+          <t>879319f127f42872ba2daeb54fc4135a</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Gasterosteus aculeatus</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Threespined stickleback</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -40228,7 +40228,7 @@
         <v>0</v>
       </c>
       <c r="AL225">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM225">
         <v>0</v>
@@ -40255,7 +40255,7 @@
         <v>0</v>
       </c>
       <c r="AU225">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV225">
         <v>0</v>
@@ -40285,17 +40285,17 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>879319f127f42872ba2daeb54fc4135a</t>
+          <t>f937641d91db232cb7180be9e04fb9e0</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Gasterosteus aculeatus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Threespined stickleback</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -40405,7 +40405,7 @@
         <v>0</v>
       </c>
       <c r="AL226">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AM226">
         <v>0</v>
@@ -40432,7 +40432,7 @@
         <v>0</v>
       </c>
       <c r="AU226">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AV226">
         <v>0</v>
@@ -40462,17 +40462,17 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>9c8a7b893d0fdaf8c1c89606cfce1c08</t>
+          <t>977b02be79d865979e54848db649eaf0</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Enchelyopus cimbrius</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Fourbeard rockling</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -40612,7 +40612,7 @@
         <v>0</v>
       </c>
       <c r="AV227">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AW227">
         <v>0</v>
@@ -40639,17 +40639,17 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>4450a6fa10b56881617cff33c5585aa8</t>
+          <t>df263dae379496c7e522db8a7dbc01c9</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Scomber scombrus</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Atlantic mackerel</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -40693,13 +40693,13 @@
         <v>0</v>
       </c>
       <c r="P228">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q228">
         <v>0</v>
       </c>
       <c r="R228">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S228">
         <v>0</v>
@@ -40714,7 +40714,7 @@
         <v>0</v>
       </c>
       <c r="W228">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X228">
         <v>0</v>
@@ -40816,17 +40816,17 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>f5ca5d430f1b145903b92fc335a4bafd</t>
+          <t>4450a6fa10b56881617cff33c5585aa8</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Lucania parva</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Rainwater killifish</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -40993,17 +40993,17 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>df263dae379496c7e522db8a7dbc01c9</t>
+          <t>f5ca5d430f1b145903b92fc335a4bafd</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Scomber scombrus</t>
+          <t>Lucania parva</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Atlantic mackerel</t>
+          <t>Rainwater killifish</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -41047,13 +41047,13 @@
         <v>0</v>
       </c>
       <c r="P230">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q230">
         <v>0</v>
       </c>
       <c r="R230">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S230">
         <v>0</v>
@@ -41068,7 +41068,7 @@
         <v>0</v>
       </c>
       <c r="W230">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X230">
         <v>0</v>
@@ -41170,17 +41170,17 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>977b02be79d865979e54848db649eaf0</t>
+          <t>9c8a7b893d0fdaf8c1c89606cfce1c08</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Enchelyopus cimbrius</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Fourbeard rockling</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -41320,7 +41320,7 @@
         <v>0</v>
       </c>
       <c r="AV231">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AW231">
         <v>0</v>
@@ -41347,17 +41347,17 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>243cc9259a8d104346a5dd517ca99499</t>
+          <t>c73c11c0d8b73d825099e12aaaefb637</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Ammodytes americanus</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>American sand lance</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -41524,17 +41524,17 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>c73c11c0d8b73d825099e12aaaefb637</t>
+          <t>c972de9c10572043855aaca4a4da68f4</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -41701,17 +41701,17 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>c972de9c10572043855aaca4a4da68f4</t>
+          <t>243cc9259a8d104346a5dd517ca99499</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Ammodytes americanus</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>American sand lance</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -43471,7 +43471,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>279fde05b5aed4bfe15ab39776ff82ba</t>
+          <t>f753730afbaa726c79bd991f32ea9778</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -43648,17 +43648,17 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>f753730afbaa726c79bd991f32ea9778</t>
+          <t>5432a6e652c21bb79c110c1179832080</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -43825,17 +43825,17 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>5432a6e652c21bb79c110c1179832080</t>
+          <t>279fde05b5aed4bfe15ab39776ff82ba</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -44179,17 +44179,17 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>88065f0fd14ae3b76fc1a87f8df6ef2d</t>
+          <t>4db280926cca07cc86b0e098513d9cc0</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -44356,22 +44356,22 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>fc6d040e1564a91e1c6d67e1e32b9022</t>
+          <t>88065f0fd14ae3b76fc1a87f8df6ef2d</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Rattus norvegicus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Norway rat</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E249">
@@ -44482,7 +44482,7 @@
         <v>0</v>
       </c>
       <c r="AN249">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AO249">
         <v>0</v>
@@ -44710,22 +44710,22 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>4db280926cca07cc86b0e098513d9cc0</t>
+          <t>fc6d040e1564a91e1c6d67e1e32b9022</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Rattus norvegicus</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Norway rat</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Mammal</t>
         </is>
       </c>
       <c r="E251">
@@ -44836,7 +44836,7 @@
         <v>0</v>
       </c>
       <c r="AN251">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AO251">
         <v>0</v>
@@ -45949,17 +45949,17 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>8103469b2716037f1cc4ce8959ae0081</t>
+          <t>14bd3bb11b9a6c641ad60556bf6141d0</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -46126,17 +46126,17 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>14bd3bb11b9a6c641ad60556bf6141d0</t>
+          <t>8103469b2716037f1cc4ce8959ae0081</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -46657,22 +46657,22 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>9dc70d19a67c006232234c9bcbbab33f</t>
+          <t>f4d5447013c09b659b99d47459de2042</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Clangula hyemalis or other Anatidae sp</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Long tailed duck or other ducks</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E262">
@@ -46780,7 +46780,7 @@
         <v>0</v>
       </c>
       <c r="AM262">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AN262">
         <v>0</v>
@@ -46834,17 +46834,17 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>f4d5447013c09b659b99d47459de2042</t>
+          <t>29d8e064f48ae7211c9fba32872b36f9</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -46957,7 +46957,7 @@
         <v>0</v>
       </c>
       <c r="AM263">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AN263">
         <v>0</v>
@@ -47011,22 +47011,22 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>29d8e064f48ae7211c9fba32872b36f9</t>
+          <t>53cfac0a209f1dbdaf758a75c84df7d6</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E264">
@@ -47188,22 +47188,22 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>53cfac0a209f1dbdaf758a75c84df7d6</t>
+          <t>9dc70d19a67c006232234c9bcbbab33f</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Clangula hyemalis or other Anatidae sp</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Long tailed duck or other ducks</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E265">
@@ -47542,7 +47542,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>4c451c35f94e737edb8816211106c35d</t>
+          <t>daa05108bed6292fbd2eedef6214fdff</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -47896,7 +47896,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>daa05108bed6292fbd2eedef6214fdff</t>
+          <t>4c451c35f94e737edb8816211106c35d</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -48073,17 +48073,17 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>26a933bf07de2306f33cc95ec94e4b2f</t>
+          <t>b61cc19540f9627af5070110979ebf91</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Pomoxis nigromaculatus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Black crappie</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -48250,17 +48250,17 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>b61cc19540f9627af5070110979ebf91</t>
+          <t>26a933bf07de2306f33cc95ec94e4b2f</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Pomoxis nigromaculatus</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Black crappie</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -48604,17 +48604,17 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>1be2860881962b4dd3a0a7c6db14ca80</t>
+          <t>93b36a6e82074114f7c4d90b6172dba2</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -48781,17 +48781,17 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>93b36a6e82074114f7c4d90b6172dba2</t>
+          <t>1be2860881962b4dd3a0a7c6db14ca80</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -49489,7 +49489,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>5cc8cf140b434a5aba3a1dad41339918</t>
+          <t>b7b35bf53a25eef31602b3f785c925e9</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -49843,7 +49843,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>b7b35bf53a25eef31602b3f785c925e9</t>
+          <t>5cc8cf140b434a5aba3a1dad41339918</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -50374,17 +50374,17 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>ed57094384d61f9a2dbc0c0e4ff6fb8a</t>
+          <t>29df87a23b45339e281dc7b390d16860</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Lepomis gibbosus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>Pumpkinseed</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -50458,7 +50458,7 @@
         <v>0</v>
       </c>
       <c r="Z283">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA283">
         <v>0</v>
@@ -50497,7 +50497,7 @@
         <v>0</v>
       </c>
       <c r="AM283">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AN283">
         <v>0</v>
@@ -50551,17 +50551,17 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>d8de668ed4c19b2b2ea845f3db18ae79</t>
+          <t>8dde047966dfd43b699a5ca7122e55d7</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Cottidae sp</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>Sculpins</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -50728,17 +50728,17 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>8dde047966dfd43b699a5ca7122e55d7</t>
+          <t>118de0da9053ad27ad0e3c1e136454d9</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -51082,17 +51082,17 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>118de0da9053ad27ad0e3c1e136454d9</t>
+          <t>ed57094384d61f9a2dbc0c0e4ff6fb8a</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Lepomis gibbosus</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Pumpkinseed</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -51166,7 +51166,7 @@
         <v>0</v>
       </c>
       <c r="Z287">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA287">
         <v>0</v>
@@ -51205,7 +51205,7 @@
         <v>0</v>
       </c>
       <c r="AM287">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AN287">
         <v>0</v>
@@ -51259,17 +51259,17 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>29df87a23b45339e281dc7b390d16860</t>
+          <t>d8de668ed4c19b2b2ea845f3db18ae79</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Cottidae sp</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Sculpins</t>
         </is>
       </c>
       <c r="D288" t="inlineStr">
@@ -51436,17 +51436,17 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>1dd0f1ca2adf649d8cba813ea6e43de2</t>
+          <t>7bb99841c9c9b86e238cbcddc0e16567</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Paralichthys dentatus</t>
+          <t>Micropterus salmoides</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>Summer flounder</t>
+          <t>Largemouth bass</t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
@@ -51967,17 +51967,17 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>7bb99841c9c9b86e238cbcddc0e16567</t>
+          <t>1dd0f1ca2adf649d8cba813ea6e43de2</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Micropterus salmoides</t>
+          <t>Paralichthys dentatus</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Largemouth bass</t>
+          <t>Summer flounder</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -52144,17 +52144,17 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>92693323f831e69117617606814ae81f</t>
+          <t>50bddde558bebcd7fa8dbf6542ea44fe</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Coryphaena hippurus</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>Mahi mahi</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
@@ -52498,17 +52498,17 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>50bddde558bebcd7fa8dbf6542ea44fe</t>
+          <t>92693323f831e69117617606814ae81f</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Coryphaena hippurus</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Mahi mahi</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
@@ -52852,17 +52852,17 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>bbd6b723329db44753870a56d15bdbd6</t>
+          <t>0d6e610cd1019f50d693803e46db364f</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Sebastes fasciatus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Acadian redfish</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
@@ -53029,17 +53029,17 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>0d6e610cd1019f50d693803e46db364f</t>
+          <t>bbd6b723329db44753870a56d15bdbd6</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Sebastes fasciatus</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Acadian redfish</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -53914,22 +53914,22 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>0a6108b3c6bbca90164970efbea23261</t>
+          <t>9f4285ab8775db6b862ee4fb416f0f5d</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Melospiza melodia or Spizella passerina</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Song sparrow or Chipping sparrow</t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E303">
@@ -53950,7 +53950,7 @@
         <v>0</v>
       </c>
       <c r="J303">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -54091,22 +54091,22 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>9f4285ab8775db6b862ee4fb416f0f5d</t>
+          <t>0a6108b3c6bbca90164970efbea23261</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Melospiza melodia or Spizella passerina</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>Song sparrow or Chipping sparrow</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E304">
@@ -54127,7 +54127,7 @@
         <v>0</v>
       </c>
       <c r="J304">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -54268,22 +54268,22 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>7950b1078efc076defba9c936b970ef7</t>
+          <t>901fc1f68af659cc3f6678c6a7396845</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E305">
@@ -54622,22 +54622,22 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>901fc1f68af659cc3f6678c6a7396845</t>
+          <t>5d4b77f374dcda6b5f48e88cc2b9664b</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E307">
@@ -54772,7 +54772,7 @@
         <v>0</v>
       </c>
       <c r="AV307">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW307">
         <v>0</v>
@@ -54799,22 +54799,22 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>5d4b77f374dcda6b5f48e88cc2b9664b</t>
+          <t>7950b1078efc076defba9c936b970ef7</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E308">
@@ -54949,7 +54949,7 @@
         <v>0</v>
       </c>
       <c r="AV308">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AW308">
         <v>0</v>
@@ -54976,17 +54976,17 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>c1f17b3dc22ac71ee83288f654c93bb3</t>
+          <t>8ea2a9236bef33ba65acfc82e6947942</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Lontra canadensis</t>
+          <t>Sciurus carolinensis</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>River otter</t>
+          <t>Gray squirrel</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
@@ -55144,7 +55144,7 @@
         <v>0</v>
       </c>
       <c r="BB309">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC309">
         <v>0</v>
@@ -55153,22 +55153,22 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>a4e8997c6347c55b72f81e0accce0c37</t>
+          <t>c1f17b3dc22ac71ee83288f654c93bb3</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Lontra canadensis</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>River otter</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Mammal</t>
         </is>
       </c>
       <c r="E310">
@@ -55330,22 +55330,22 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>8ea2a9236bef33ba65acfc82e6947942</t>
+          <t>a4e8997c6347c55b72f81e0accce0c37</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Sciurus carolinensis</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>Gray squirrel</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E311">
@@ -55498,7 +55498,7 @@
         <v>0</v>
       </c>
       <c r="BB311">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC311">
         <v>0</v>
@@ -55684,17 +55684,17 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>16d55edf1062cb60bf8a36a1da3212b5</t>
+          <t>7eef5797ad87b51600785f22606c70de</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Esox americanus or niger</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>Grass or chain pickerel</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -55831,7 +55831,7 @@
         <v>0</v>
       </c>
       <c r="AU313">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AV313">
         <v>0</v>
@@ -55861,17 +55861,17 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>7eef5797ad87b51600785f22606c70de</t>
+          <t>033531a8711295f5cf38c1111629eb77</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Anguilla rostrata</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>American eel</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
@@ -56215,17 +56215,17 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>5b1dbdcc719bcfd9ea209ec7d9ecd075</t>
+          <t>16d55edf1062cb60bf8a36a1da3212b5</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Esox americanus or niger</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Grass or chain pickerel</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
@@ -56362,7 +56362,7 @@
         <v>0</v>
       </c>
       <c r="AU316">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AV316">
         <v>0</v>
@@ -56392,17 +56392,17 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>033531a8711295f5cf38c1111629eb77</t>
+          <t>5b1dbdcc719bcfd9ea209ec7d9ecd075</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Anguilla rostrata</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>American eel</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
@@ -56746,22 +56746,22 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>bfab25a003878187c8038ee55fdb7a53</t>
+          <t>d1de955bd9480b3f0c70f78caec5a443</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Gavia immer</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>Common loon</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E319">
@@ -56923,22 +56923,22 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>d1de955bd9480b3f0c70f78caec5a443</t>
+          <t>bfab25a003878187c8038ee55fdb7a53</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Gavia immer</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Common loon</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E320">
@@ -57100,22 +57100,22 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>9ed3306f1d1dfb81749820128e325abc</t>
+          <t>fb3bb0a4483dcfbc39e8b7ccf8196749</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E321">
@@ -57277,22 +57277,22 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>fb3bb0a4483dcfbc39e8b7ccf8196749</t>
+          <t>9ed3306f1d1dfb81749820128e325abc</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E322">
@@ -58162,22 +58162,22 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>032747b5e01bbdc74f3e3e59d9c2275f</t>
+          <t>9f2355fd161fec0177a83045e771a239</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Decapterus punctatus</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Round scad</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E327">
@@ -58339,22 +58339,22 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>9f2355fd161fec0177a83045e771a239</t>
+          <t>032747b5e01bbdc74f3e3e59d9c2275f</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Decapterus punctatus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>Round scad</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E328">
@@ -59755,17 +59755,17 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>38e4381a618398d035b19d8c47e8bfa3</t>
+          <t>856a99622e9c49fc86cdcf3ddbefcfd1</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Gobiosoma ginsburgi</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Seaboard goby</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
@@ -59932,17 +59932,17 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>856a99622e9c49fc86cdcf3ddbefcfd1</t>
+          <t>38e4381a618398d035b19d8c47e8bfa3</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Gobiosoma ginsburgi</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>Seaboard goby</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -60109,22 +60109,22 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>d3b57d4cf93def7c41d4b9baced940d9</t>
+          <t>a1f66fcba0bd12eed7a60901bd8c6010</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Canis lupus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E338">
@@ -60463,17 +60463,17 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>a1f66fcba0bd12eed7a60901bd8c6010</t>
+          <t>5cde257b7febb75f7c9848a21bfe18cd</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
@@ -60640,22 +60640,22 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>5cde257b7febb75f7c9848a21bfe18cd</t>
+          <t>d3b57d4cf93def7c41d4b9baced940d9</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Canis lupus</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E341">
@@ -60994,17 +60994,17 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>e7f90ff8c7b97da66ce6d940d857e8e4</t>
+          <t>60fb36f888cbf7e4639c1bb98f0adc57</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Trachurus lathami</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>Rough scad</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
@@ -61348,17 +61348,17 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>60fb36f888cbf7e4639c1bb98f0adc57</t>
+          <t>e7f90ff8c7b97da66ce6d940d857e8e4</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Trachurus lathami</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Rough scad</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
@@ -61525,22 +61525,22 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>7fef2f8e6a8bee56528216dfc05f0d81</t>
+          <t>bcf13bc540e00c02358754d8a1b40a9c</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E346">
@@ -61702,22 +61702,22 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>bcf13bc540e00c02358754d8a1b40a9c</t>
+          <t>7fef2f8e6a8bee56528216dfc05f0d81</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E347">
@@ -62764,17 +62764,17 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>35a8484c22fbf1df676003af6ec52a29</t>
+          <t>1a9a786e8451eec71300762a5398f4d0</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Anguilla rostrata</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>American eel</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
@@ -62941,22 +62941,22 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>1a9a786e8451eec71300762a5398f4d0</t>
+          <t>0e3aec812235602fac414c57ef969f1e</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Anguilla rostrata</t>
+          <t>Peromyscus leucopus</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>American eel</t>
+          <t>Deer mouse</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Mammal</t>
         </is>
       </c>
       <c r="E354">
@@ -63088,7 +63088,7 @@
         <v>0</v>
       </c>
       <c r="AU354">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV354">
         <v>0</v>
@@ -63112,28 +63112,28 @@
         <v>0</v>
       </c>
       <c r="BC354">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>0e3aec812235602fac414c57ef969f1e</t>
+          <t>35a8484c22fbf1df676003af6ec52a29</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Peromyscus leucopus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>Deer mouse</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E355">
@@ -63265,7 +63265,7 @@
         <v>0</v>
       </c>
       <c r="AU355">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV355">
         <v>0</v>
@@ -63289,23 +63289,23 @@
         <v>0</v>
       </c>
       <c r="BC355">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>b45f5a79f080475521114b63aa9bd7d1</t>
+          <t>841570d820eaab46bb7c7b3b7db8fba3</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Thunnus sp</t>
+          <t>Ctenogobius boleosoma</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>Tuna sp</t>
+          <t>Darter goby</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
@@ -63472,22 +63472,22 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>cc23248fc9f0058810041c6090c99461</t>
+          <t>b45f5a79f080475521114b63aa9bd7d1</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Thunnus sp</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Tuna sp</t>
         </is>
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E357">
@@ -63649,17 +63649,17 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>841570d820eaab46bb7c7b3b7db8fba3</t>
+          <t>5d6bb2fed75f92f01e645ffc80d17d36</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Ctenogobius boleosoma</t>
+          <t>Anchoa mitchilli</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>Darter goby</t>
+          <t>Bay anchovy</t>
         </is>
       </c>
       <c r="D358" t="inlineStr">
@@ -63826,22 +63826,22 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>5d6bb2fed75f92f01e645ffc80d17d36</t>
+          <t>cc23248fc9f0058810041c6090c99461</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>Anchoa mitchilli</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>Bay anchovy</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E359">
@@ -64711,7 +64711,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>0dc4976a75f5949215d7cf1f1a2994f6</t>
+          <t>02af37069efe14191838e3ded56eba42</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -64888,22 +64888,22 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>dedc23ac2bedc9a49f0d9d5f2092f08a</t>
+          <t>0dc4976a75f5949215d7cf1f1a2994f6</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>Sternotherus carinatus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>Razor-backed musk turtle</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Reptile</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E365">
@@ -65038,7 +65038,7 @@
         <v>0</v>
       </c>
       <c r="AV365">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AW365">
         <v>0</v>
@@ -65065,22 +65065,22 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>02af37069efe14191838e3ded56eba42</t>
+          <t>dedc23ac2bedc9a49f0d9d5f2092f08a</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Sternotherus carinatus</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Razor-backed musk turtle</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Reptile</t>
         </is>
       </c>
       <c r="E366">
@@ -65215,7 +65215,7 @@
         <v>0</v>
       </c>
       <c r="AV366">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW366">
         <v>0</v>
@@ -65419,22 +65419,22 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>f3ca4711d94796503be4e5bbb8a6705b</t>
+          <t>072eff78dfd4d6ee7d89b57c63c82827</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Cottidae sp</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Sculpins</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E368">
@@ -65515,7 +65515,7 @@
         <v>0</v>
       </c>
       <c r="AD368">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE368">
         <v>0</v>
@@ -65542,7 +65542,7 @@
         <v>0</v>
       </c>
       <c r="AM368">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AN368">
         <v>0</v>
@@ -65596,22 +65596,22 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>072eff78dfd4d6ee7d89b57c63c82827</t>
+          <t>f3ca4711d94796503be4e5bbb8a6705b</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Cottidae sp</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>Sculpins</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E369">
@@ -65692,7 +65692,7 @@
         <v>0</v>
       </c>
       <c r="AD369">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE369">
         <v>0</v>
@@ -65719,7 +65719,7 @@
         <v>0</v>
       </c>
       <c r="AM369">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN369">
         <v>0</v>
@@ -66835,7 +66835,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>9b1cbc97eff7dc6af2c100d85526140f</t>
+          <t>66ce172600ad7ff5f35d5dfc0bab87d3</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -66895,7 +66895,7 @@
         <v>0</v>
       </c>
       <c r="R376">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S376">
         <v>0</v>
@@ -66958,7 +66958,7 @@
         <v>0</v>
       </c>
       <c r="AM376">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AN376">
         <v>0</v>
@@ -66967,7 +66967,7 @@
         <v>0</v>
       </c>
       <c r="AP376">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ376">
         <v>0</v>
@@ -67006,13 +67006,13 @@
         <v>0</v>
       </c>
       <c r="BC376">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>66ce172600ad7ff5f35d5dfc0bab87d3</t>
+          <t>9b1cbc97eff7dc6af2c100d85526140f</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -67072,7 +67072,7 @@
         <v>0</v>
       </c>
       <c r="R377">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S377">
         <v>0</v>
@@ -67135,7 +67135,7 @@
         <v>0</v>
       </c>
       <c r="AM377">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AN377">
         <v>0</v>
@@ -67144,7 +67144,7 @@
         <v>0</v>
       </c>
       <c r="AP377">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ377">
         <v>0</v>
@@ -67183,7 +67183,7 @@
         <v>0</v>
       </c>
       <c r="BC377">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378">
@@ -67543,22 +67543,22 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>97444d2388851f1d71afeb95125b4898</t>
+          <t>798cab8e6a1a556a317f78cfa6bab8ac</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Felis catus</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E380">
@@ -67720,22 +67720,22 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>798cab8e6a1a556a317f78cfa6bab8ac</t>
+          <t>97444d2388851f1d71afeb95125b4898</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Felis catus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E381">
@@ -68782,22 +68782,22 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>3b578403acdc73dd077d282c96f9541f</t>
+          <t>41714252fc55bbced79f657eb2b8805a</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Ophidion marginatum</t>
+          <t>Passer domesticus</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>Striped cusk-eel</t>
+          <t>House sparrow</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E387">
@@ -68911,13 +68911,13 @@
         <v>0</v>
       </c>
       <c r="AO387">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AP387">
         <v>0</v>
       </c>
       <c r="AQ387">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AR387">
         <v>0</v>
@@ -68932,22 +68932,22 @@
         <v>0</v>
       </c>
       <c r="AV387">
+        <v>0</v>
+      </c>
+      <c r="AW387">
+        <v>0</v>
+      </c>
+      <c r="AX387">
+        <v>0</v>
+      </c>
+      <c r="AY387">
+        <v>0</v>
+      </c>
+      <c r="AZ387">
+        <v>0</v>
+      </c>
+      <c r="BA387">
         <v>5</v>
-      </c>
-      <c r="AW387">
-        <v>0</v>
-      </c>
-      <c r="AX387">
-        <v>0</v>
-      </c>
-      <c r="AY387">
-        <v>0</v>
-      </c>
-      <c r="AZ387">
-        <v>0</v>
-      </c>
-      <c r="BA387">
-        <v>0</v>
       </c>
       <c r="BB387">
         <v>0</v>
@@ -69136,22 +69136,22 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>41714252fc55bbced79f657eb2b8805a</t>
+          <t>3b578403acdc73dd077d282c96f9541f</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Passer domesticus</t>
+          <t>Ophidion marginatum</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>House sparrow</t>
+          <t>Striped cusk-eel</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E389">
@@ -69265,13 +69265,13 @@
         <v>0</v>
       </c>
       <c r="AO389">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AP389">
         <v>0</v>
       </c>
       <c r="AQ389">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AR389">
         <v>0</v>
@@ -69286,7 +69286,7 @@
         <v>0</v>
       </c>
       <c r="AV389">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW389">
         <v>0</v>
@@ -69301,7 +69301,7 @@
         <v>0</v>
       </c>
       <c r="BA389">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BB389">
         <v>0</v>
@@ -69844,22 +69844,22 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>803a43fa7cb74bb51f36ab2949523bf2</t>
+          <t>d1af29b8548fccd9f3eada2b18f0eac9</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E393">
@@ -70021,22 +70021,22 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>812ed0386e2a4869a21da5634665548d</t>
+          <t>803a43fa7cb74bb51f36ab2949523bf2</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Caranx hippos</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>Crevalle jack</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E394">
@@ -70552,22 +70552,22 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>d1af29b8548fccd9f3eada2b18f0eac9</t>
+          <t>812ed0386e2a4869a21da5634665548d</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Caranx hippos</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Crevalle jack</t>
         </is>
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E397">
@@ -71791,22 +71791,22 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>2d0506c060ee125f6608b52f22e598b1</t>
+          <t>a6bf1361741b5eda21b4d05f18f04a90</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E404">
@@ -71941,25 +71941,25 @@
         <v>0</v>
       </c>
       <c r="AV404">
+        <v>0</v>
+      </c>
+      <c r="AW404">
+        <v>0</v>
+      </c>
+      <c r="AX404">
+        <v>0</v>
+      </c>
+      <c r="AY404">
+        <v>0</v>
+      </c>
+      <c r="AZ404">
+        <v>0</v>
+      </c>
+      <c r="BA404">
+        <v>0</v>
+      </c>
+      <c r="BB404">
         <v>8</v>
-      </c>
-      <c r="AW404">
-        <v>0</v>
-      </c>
-      <c r="AX404">
-        <v>0</v>
-      </c>
-      <c r="AY404">
-        <v>0</v>
-      </c>
-      <c r="AZ404">
-        <v>0</v>
-      </c>
-      <c r="BA404">
-        <v>0</v>
-      </c>
-      <c r="BB404">
-        <v>0</v>
       </c>
       <c r="BC404">
         <v>0</v>
@@ -71968,22 +71968,22 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>a6bf1361741b5eda21b4d05f18f04a90</t>
+          <t>2d0506c060ee125f6608b52f22e598b1</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E405">
@@ -72118,7 +72118,7 @@
         <v>0</v>
       </c>
       <c r="AV405">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AW405">
         <v>0</v>
@@ -72136,7 +72136,7 @@
         <v>0</v>
       </c>
       <c r="BB405">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BC405">
         <v>0</v>
@@ -72322,22 +72322,22 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>037bd6992d173dfbcd22d76af622fa5b</t>
+          <t>9e218ddde05826daea9943de26124674</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Malaclemys terrapin</t>
+          <t>Sturnus vulgaris</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>Diamondback terrapin</t>
+          <t>Common starling</t>
         </is>
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>Reptile</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E407">
@@ -72412,67 +72412,67 @@
         <v>0</v>
       </c>
       <c r="AB407">
+        <v>0</v>
+      </c>
+      <c r="AC407">
+        <v>0</v>
+      </c>
+      <c r="AD407">
+        <v>0</v>
+      </c>
+      <c r="AE407">
+        <v>0</v>
+      </c>
+      <c r="AF407">
+        <v>0</v>
+      </c>
+      <c r="AG407">
+        <v>0</v>
+      </c>
+      <c r="AH407">
+        <v>0</v>
+      </c>
+      <c r="AI407">
+        <v>0</v>
+      </c>
+      <c r="AJ407">
+        <v>0</v>
+      </c>
+      <c r="AK407">
+        <v>0</v>
+      </c>
+      <c r="AL407">
+        <v>0</v>
+      </c>
+      <c r="AM407">
+        <v>0</v>
+      </c>
+      <c r="AN407">
+        <v>0</v>
+      </c>
+      <c r="AO407">
+        <v>0</v>
+      </c>
+      <c r="AP407">
+        <v>0</v>
+      </c>
+      <c r="AQ407">
+        <v>0</v>
+      </c>
+      <c r="AR407">
+        <v>0</v>
+      </c>
+      <c r="AS407">
+        <v>0</v>
+      </c>
+      <c r="AT407">
+        <v>0</v>
+      </c>
+      <c r="AU407">
+        <v>0</v>
+      </c>
+      <c r="AV407">
         <v>7</v>
-      </c>
-      <c r="AC407">
-        <v>0</v>
-      </c>
-      <c r="AD407">
-        <v>0</v>
-      </c>
-      <c r="AE407">
-        <v>0</v>
-      </c>
-      <c r="AF407">
-        <v>0</v>
-      </c>
-      <c r="AG407">
-        <v>0</v>
-      </c>
-      <c r="AH407">
-        <v>0</v>
-      </c>
-      <c r="AI407">
-        <v>0</v>
-      </c>
-      <c r="AJ407">
-        <v>0</v>
-      </c>
-      <c r="AK407">
-        <v>0</v>
-      </c>
-      <c r="AL407">
-        <v>0</v>
-      </c>
-      <c r="AM407">
-        <v>0</v>
-      </c>
-      <c r="AN407">
-        <v>0</v>
-      </c>
-      <c r="AO407">
-        <v>0</v>
-      </c>
-      <c r="AP407">
-        <v>0</v>
-      </c>
-      <c r="AQ407">
-        <v>0</v>
-      </c>
-      <c r="AR407">
-        <v>0</v>
-      </c>
-      <c r="AS407">
-        <v>0</v>
-      </c>
-      <c r="AT407">
-        <v>0</v>
-      </c>
-      <c r="AU407">
-        <v>0</v>
-      </c>
-      <c r="AV407">
-        <v>0</v>
       </c>
       <c r="AW407">
         <v>0</v>
@@ -72499,17 +72499,17 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>75fedd0fa34e3ac2514601e68b613736</t>
+          <t>f6b3a673a06591a2d5a8936584e64754</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Strongylura marina</t>
+          <t>Tautogolabrus adspersus</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>Atlantic needlefish</t>
+          <t>Cunner</t>
         </is>
       </c>
       <c r="D408" t="inlineStr">
@@ -72601,52 +72601,52 @@
         <v>0</v>
       </c>
       <c r="AF408">
+        <v>0</v>
+      </c>
+      <c r="AG408">
+        <v>0</v>
+      </c>
+      <c r="AH408">
+        <v>0</v>
+      </c>
+      <c r="AI408">
+        <v>0</v>
+      </c>
+      <c r="AJ408">
+        <v>0</v>
+      </c>
+      <c r="AK408">
+        <v>0</v>
+      </c>
+      <c r="AL408">
+        <v>0</v>
+      </c>
+      <c r="AM408">
+        <v>0</v>
+      </c>
+      <c r="AN408">
+        <v>0</v>
+      </c>
+      <c r="AO408">
+        <v>0</v>
+      </c>
+      <c r="AP408">
+        <v>0</v>
+      </c>
+      <c r="AQ408">
+        <v>0</v>
+      </c>
+      <c r="AR408">
+        <v>0</v>
+      </c>
+      <c r="AS408">
+        <v>0</v>
+      </c>
+      <c r="AT408">
+        <v>0</v>
+      </c>
+      <c r="AU408">
         <v>7</v>
-      </c>
-      <c r="AG408">
-        <v>0</v>
-      </c>
-      <c r="AH408">
-        <v>0</v>
-      </c>
-      <c r="AI408">
-        <v>0</v>
-      </c>
-      <c r="AJ408">
-        <v>0</v>
-      </c>
-      <c r="AK408">
-        <v>0</v>
-      </c>
-      <c r="AL408">
-        <v>0</v>
-      </c>
-      <c r="AM408">
-        <v>0</v>
-      </c>
-      <c r="AN408">
-        <v>0</v>
-      </c>
-      <c r="AO408">
-        <v>0</v>
-      </c>
-      <c r="AP408">
-        <v>0</v>
-      </c>
-      <c r="AQ408">
-        <v>0</v>
-      </c>
-      <c r="AR408">
-        <v>0</v>
-      </c>
-      <c r="AS408">
-        <v>0</v>
-      </c>
-      <c r="AT408">
-        <v>0</v>
-      </c>
-      <c r="AU408">
-        <v>0</v>
       </c>
       <c r="AV408">
         <v>0</v>
@@ -72676,17 +72676,17 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>f6b3a673a06591a2d5a8936584e64754</t>
+          <t>75fedd0fa34e3ac2514601e68b613736</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Tautogolabrus adspersus</t>
+          <t>Strongylura marina</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>Cunner</t>
+          <t>Atlantic needlefish</t>
         </is>
       </c>
       <c r="D409" t="inlineStr">
@@ -72778,7 +72778,7 @@
         <v>0</v>
       </c>
       <c r="AF409">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG409">
         <v>0</v>
@@ -72823,7 +72823,7 @@
         <v>0</v>
       </c>
       <c r="AU409">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AV409">
         <v>0</v>
@@ -73030,22 +73030,22 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>08bd987bd944513cc896ab3b3c3eed38</t>
+          <t>037bd6992d173dfbcd22d76af622fa5b</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Hippoglossina oblonga</t>
+          <t>Malaclemys terrapin</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>Fourspot flounder</t>
+          <t>Diamondback terrapin</t>
         </is>
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Reptile</t>
         </is>
       </c>
       <c r="E411">
@@ -73120,7 +73120,7 @@
         <v>0</v>
       </c>
       <c r="AB411">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC411">
         <v>0</v>
@@ -73162,7 +73162,7 @@
         <v>0</v>
       </c>
       <c r="AP411">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AQ411">
         <v>0</v>
@@ -73207,22 +73207,22 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>9e218ddde05826daea9943de26124674</t>
+          <t>08bd987bd944513cc896ab3b3c3eed38</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Sturnus vulgaris</t>
+          <t>Hippoglossina oblonga</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>Common starling</t>
+          <t>Fourspot flounder</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E412">
@@ -73339,7 +73339,7 @@
         <v>0</v>
       </c>
       <c r="AP412">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AQ412">
         <v>0</v>
@@ -73357,7 +73357,7 @@
         <v>0</v>
       </c>
       <c r="AV412">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AW412">
         <v>0</v>
@@ -73384,22 +73384,22 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>ced5f183dc83bf9a3831984cefa3b3a1</t>
+          <t>0437f2363acf453d6291ceda4abba683</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Ameiurus nebulosus</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Brown bullhead</t>
         </is>
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E413">
@@ -73474,7 +73474,7 @@
         <v>0</v>
       </c>
       <c r="AB413">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AC413">
         <v>0</v>
@@ -73549,7 +73549,7 @@
         <v>0</v>
       </c>
       <c r="BA413">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BB413">
         <v>0</v>
@@ -73561,22 +73561,22 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>d964add43fe0c3212cbe19a066dc2a13</t>
+          <t>956d5064b9d6c222e19d75e231925e18</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E414">
@@ -73621,7 +73621,7 @@
         <v>0</v>
       </c>
       <c r="R414">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S414">
         <v>0</v>
@@ -73732,28 +73732,28 @@
         <v>0</v>
       </c>
       <c r="BC414">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>956d5064b9d6c222e19d75e231925e18</t>
+          <t>d964add43fe0c3212cbe19a066dc2a13</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E415">
@@ -73798,134 +73798,134 @@
         <v>0</v>
       </c>
       <c r="R415">
+        <v>0</v>
+      </c>
+      <c r="S415">
+        <v>0</v>
+      </c>
+      <c r="T415">
+        <v>0</v>
+      </c>
+      <c r="U415">
+        <v>0</v>
+      </c>
+      <c r="V415">
+        <v>0</v>
+      </c>
+      <c r="W415">
+        <v>0</v>
+      </c>
+      <c r="X415">
+        <v>0</v>
+      </c>
+      <c r="Y415">
+        <v>0</v>
+      </c>
+      <c r="Z415">
+        <v>0</v>
+      </c>
+      <c r="AA415">
+        <v>0</v>
+      </c>
+      <c r="AB415">
+        <v>0</v>
+      </c>
+      <c r="AC415">
+        <v>0</v>
+      </c>
+      <c r="AD415">
+        <v>0</v>
+      </c>
+      <c r="AE415">
+        <v>0</v>
+      </c>
+      <c r="AF415">
+        <v>0</v>
+      </c>
+      <c r="AG415">
+        <v>0</v>
+      </c>
+      <c r="AH415">
+        <v>0</v>
+      </c>
+      <c r="AI415">
+        <v>0</v>
+      </c>
+      <c r="AJ415">
+        <v>0</v>
+      </c>
+      <c r="AK415">
+        <v>0</v>
+      </c>
+      <c r="AL415">
+        <v>0</v>
+      </c>
+      <c r="AM415">
+        <v>0</v>
+      </c>
+      <c r="AN415">
+        <v>0</v>
+      </c>
+      <c r="AO415">
+        <v>0</v>
+      </c>
+      <c r="AP415">
+        <v>0</v>
+      </c>
+      <c r="AQ415">
+        <v>0</v>
+      </c>
+      <c r="AR415">
+        <v>0</v>
+      </c>
+      <c r="AS415">
+        <v>0</v>
+      </c>
+      <c r="AT415">
+        <v>0</v>
+      </c>
+      <c r="AU415">
+        <v>0</v>
+      </c>
+      <c r="AV415">
+        <v>0</v>
+      </c>
+      <c r="AW415">
+        <v>0</v>
+      </c>
+      <c r="AX415">
+        <v>0</v>
+      </c>
+      <c r="AY415">
+        <v>0</v>
+      </c>
+      <c r="AZ415">
+        <v>0</v>
+      </c>
+      <c r="BA415">
+        <v>0</v>
+      </c>
+      <c r="BB415">
+        <v>0</v>
+      </c>
+      <c r="BC415">
         <v>6</v>
-      </c>
-      <c r="S415">
-        <v>0</v>
-      </c>
-      <c r="T415">
-        <v>0</v>
-      </c>
-      <c r="U415">
-        <v>0</v>
-      </c>
-      <c r="V415">
-        <v>0</v>
-      </c>
-      <c r="W415">
-        <v>0</v>
-      </c>
-      <c r="X415">
-        <v>0</v>
-      </c>
-      <c r="Y415">
-        <v>0</v>
-      </c>
-      <c r="Z415">
-        <v>0</v>
-      </c>
-      <c r="AA415">
-        <v>0</v>
-      </c>
-      <c r="AB415">
-        <v>0</v>
-      </c>
-      <c r="AC415">
-        <v>0</v>
-      </c>
-      <c r="AD415">
-        <v>0</v>
-      </c>
-      <c r="AE415">
-        <v>0</v>
-      </c>
-      <c r="AF415">
-        <v>0</v>
-      </c>
-      <c r="AG415">
-        <v>0</v>
-      </c>
-      <c r="AH415">
-        <v>0</v>
-      </c>
-      <c r="AI415">
-        <v>0</v>
-      </c>
-      <c r="AJ415">
-        <v>0</v>
-      </c>
-      <c r="AK415">
-        <v>0</v>
-      </c>
-      <c r="AL415">
-        <v>0</v>
-      </c>
-      <c r="AM415">
-        <v>0</v>
-      </c>
-      <c r="AN415">
-        <v>0</v>
-      </c>
-      <c r="AO415">
-        <v>0</v>
-      </c>
-      <c r="AP415">
-        <v>0</v>
-      </c>
-      <c r="AQ415">
-        <v>0</v>
-      </c>
-      <c r="AR415">
-        <v>0</v>
-      </c>
-      <c r="AS415">
-        <v>0</v>
-      </c>
-      <c r="AT415">
-        <v>0</v>
-      </c>
-      <c r="AU415">
-        <v>0</v>
-      </c>
-      <c r="AV415">
-        <v>0</v>
-      </c>
-      <c r="AW415">
-        <v>0</v>
-      </c>
-      <c r="AX415">
-        <v>0</v>
-      </c>
-      <c r="AY415">
-        <v>0</v>
-      </c>
-      <c r="AZ415">
-        <v>0</v>
-      </c>
-      <c r="BA415">
-        <v>0</v>
-      </c>
-      <c r="BB415">
-        <v>0</v>
-      </c>
-      <c r="BC415">
-        <v>0</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>0437f2363acf453d6291ceda4abba683</t>
+          <t>7f400300a06f165c23af04aa4e4c790c</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Ameiurus nebulosus</t>
+          <t>Enchelyopus cimbrius</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>Brown bullhead</t>
+          <t>Fourbeard rockling</t>
         </is>
       </c>
       <c r="D416" t="inlineStr">
@@ -74005,40 +74005,40 @@
         <v>0</v>
       </c>
       <c r="AB416">
+        <v>0</v>
+      </c>
+      <c r="AC416">
+        <v>0</v>
+      </c>
+      <c r="AD416">
+        <v>0</v>
+      </c>
+      <c r="AE416">
+        <v>0</v>
+      </c>
+      <c r="AF416">
+        <v>0</v>
+      </c>
+      <c r="AG416">
+        <v>0</v>
+      </c>
+      <c r="AH416">
+        <v>0</v>
+      </c>
+      <c r="AI416">
+        <v>0</v>
+      </c>
+      <c r="AJ416">
+        <v>0</v>
+      </c>
+      <c r="AK416">
+        <v>0</v>
+      </c>
+      <c r="AL416">
+        <v>0</v>
+      </c>
+      <c r="AM416">
         <v>6</v>
-      </c>
-      <c r="AC416">
-        <v>0</v>
-      </c>
-      <c r="AD416">
-        <v>0</v>
-      </c>
-      <c r="AE416">
-        <v>0</v>
-      </c>
-      <c r="AF416">
-        <v>0</v>
-      </c>
-      <c r="AG416">
-        <v>0</v>
-      </c>
-      <c r="AH416">
-        <v>0</v>
-      </c>
-      <c r="AI416">
-        <v>0</v>
-      </c>
-      <c r="AJ416">
-        <v>0</v>
-      </c>
-      <c r="AK416">
-        <v>0</v>
-      </c>
-      <c r="AL416">
-        <v>0</v>
-      </c>
-      <c r="AM416">
-        <v>0</v>
       </c>
       <c r="AN416">
         <v>0</v>
@@ -74092,22 +74092,22 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>29ae99676d91135240ab43f0184c5909</t>
+          <t>ced5f183dc83bf9a3831984cefa3b3a1</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E417">
@@ -74242,22 +74242,22 @@
         <v>0</v>
       </c>
       <c r="AV417">
+        <v>0</v>
+      </c>
+      <c r="AW417">
+        <v>0</v>
+      </c>
+      <c r="AX417">
+        <v>0</v>
+      </c>
+      <c r="AY417">
+        <v>0</v>
+      </c>
+      <c r="AZ417">
+        <v>0</v>
+      </c>
+      <c r="BA417">
         <v>6</v>
-      </c>
-      <c r="AW417">
-        <v>0</v>
-      </c>
-      <c r="AX417">
-        <v>0</v>
-      </c>
-      <c r="AY417">
-        <v>0</v>
-      </c>
-      <c r="AZ417">
-        <v>0</v>
-      </c>
-      <c r="BA417">
-        <v>0</v>
       </c>
       <c r="BB417">
         <v>0</v>
@@ -74269,22 +74269,22 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>7f400300a06f165c23af04aa4e4c790c</t>
+          <t>29ae99676d91135240ab43f0184c5909</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Enchelyopus cimbrius</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>Fourbeard rockling</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E418">
@@ -74392,34 +74392,34 @@
         <v>0</v>
       </c>
       <c r="AM418">
+        <v>0</v>
+      </c>
+      <c r="AN418">
+        <v>0</v>
+      </c>
+      <c r="AO418">
+        <v>0</v>
+      </c>
+      <c r="AP418">
+        <v>0</v>
+      </c>
+      <c r="AQ418">
+        <v>0</v>
+      </c>
+      <c r="AR418">
+        <v>0</v>
+      </c>
+      <c r="AS418">
+        <v>0</v>
+      </c>
+      <c r="AT418">
+        <v>0</v>
+      </c>
+      <c r="AU418">
+        <v>0</v>
+      </c>
+      <c r="AV418">
         <v>6</v>
-      </c>
-      <c r="AN418">
-        <v>0</v>
-      </c>
-      <c r="AO418">
-        <v>0</v>
-      </c>
-      <c r="AP418">
-        <v>0</v>
-      </c>
-      <c r="AQ418">
-        <v>0</v>
-      </c>
-      <c r="AR418">
-        <v>0</v>
-      </c>
-      <c r="AS418">
-        <v>0</v>
-      </c>
-      <c r="AT418">
-        <v>0</v>
-      </c>
-      <c r="AU418">
-        <v>0</v>
-      </c>
-      <c r="AV418">
-        <v>0</v>
       </c>
       <c r="AW418">
         <v>0</v>
@@ -74446,22 +74446,22 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>39c09623e77e6cb1f69a264089e6256c</t>
+          <t>df6846357baa6a9fecd66b4a1ba513a8</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Blarina brevicauda</t>
+          <t>Canis lupus</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>Northern short tailed shrew</t>
+          <t>Dog</t>
         </is>
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>Mammal</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E419">
@@ -74476,13 +74476,13 @@
         <v>0</v>
       </c>
       <c r="H419">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I419">
         <v>0</v>
       </c>
       <c r="J419">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K419">
         <v>0</v>
@@ -74623,22 +74623,22 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>df6846357baa6a9fecd66b4a1ba513a8</t>
+          <t>39c09623e77e6cb1f69a264089e6256c</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Canis lupus</t>
+          <t>Blarina brevicauda</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>Dog</t>
+          <t>Northern short tailed shrew</t>
         </is>
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Mammal</t>
         </is>
       </c>
       <c r="E420">
@@ -74653,13 +74653,13 @@
         <v>0</v>
       </c>
       <c r="H420">
+        <v>0</v>
+      </c>
+      <c r="I420">
+        <v>0</v>
+      </c>
+      <c r="J420">
         <v>5</v>
-      </c>
-      <c r="I420">
-        <v>0</v>
-      </c>
-      <c r="J420">
-        <v>0</v>
       </c>
       <c r="K420">
         <v>0</v>

</xml_diff>